<commit_message>
updated master data and setup python
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Belize\IJ-CODE\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6ACF9C6-CD0E-4649-B0AC-26C76F66FCC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F907A8E-1C02-46A2-BDC3-ADC0F0F66C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -192,7 +192,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,12 +508,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.44140625" style="1"/>
     <col min="5" max="5" width="8.5546875" style="1"/>
   </cols>
@@ -537,16 +535,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -554,16 +552,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -571,16 +569,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -588,16 +586,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -605,16 +603,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -622,16 +620,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -639,16 +637,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -656,16 +654,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -673,16 +671,16 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -690,16 +688,16 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -707,16 +705,16 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -724,16 +722,16 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -741,16 +739,16 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -758,16 +756,16 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -775,16 +773,16 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -792,16 +790,16 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -809,16 +807,16 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -826,16 +824,16 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -843,16 +841,16 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" t="s">
         <v>13</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -860,16 +858,16 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -877,16 +875,16 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="A22" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -894,16 +892,16 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -911,16 +909,16 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" t="s">
         <v>13</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -928,16 +926,16 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -945,16 +943,16 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="A26" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" t="s">
         <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -962,16 +960,16 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="A27" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -979,16 +977,16 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -996,16 +994,16 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" t="s">
         <v>13</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -1013,16 +1011,16 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -1030,16 +1028,16 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="A31" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" t="s">
         <v>11</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -1047,16 +1045,16 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" t="s">
         <v>13</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -1064,16 +1062,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="A33" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" t="s">
         <v>15</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -1081,16 +1079,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="A34" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" t="s">
         <v>25</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -1098,16 +1096,16 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" t="s">
         <v>7</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -1115,16 +1113,16 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" t="s">
         <v>11</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1132,16 +1130,16 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="A37" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C37" t="s">
         <v>12</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" t="s">
         <v>13</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -1149,16 +1147,16 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" t="s">
         <v>25</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -1166,16 +1164,16 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -1183,16 +1181,16 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" t="s">
         <v>12</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" t="s">
         <v>13</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -1200,16 +1198,16 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" t="s">
         <v>15</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -1217,16 +1215,16 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" t="s">
         <v>25</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -1234,16 +1232,16 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="A43" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" t="s">
         <v>7</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -1251,16 +1249,16 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="D44" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -1268,16 +1266,16 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" t="s">
         <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" t="s">
         <v>25</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -1285,16 +1283,16 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" t="s">
         <v>7</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -1302,16 +1300,16 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -1319,16 +1317,16 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="A48" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" t="s">
         <v>13</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -1336,16 +1334,16 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="A49" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C49" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" t="s">
         <v>15</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -1353,16 +1351,16 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="A50" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="D50" t="s">
         <v>25</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -1370,16 +1368,16 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" t="s">
         <v>7</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -1387,16 +1385,16 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" t="s">
         <v>10</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="D52" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -1404,16 +1402,16 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="A53" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="C53" t="s">
         <v>12</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="D53" t="s">
         <v>13</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -1421,16 +1419,16 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+      <c r="A54" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="4" t="s">
+      <c r="D54" t="s">
         <v>25</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -1438,16 +1436,16 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+      <c r="A55" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C55" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="4" t="s">
+      <c r="D55" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -1455,16 +1453,16 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="A56" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" t="s">
         <v>12</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" t="s">
         <v>13</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -1472,16 +1470,16 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+      <c r="A57" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" t="s">
         <v>15</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -1489,16 +1487,16 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+      <c r="A58" t="s">
         <v>5</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" t="s">
         <v>24</v>
       </c>
-      <c r="D58" s="4" t="s">
+      <c r="D58" t="s">
         <v>25</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -1506,16 +1504,16 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="A59" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="C59" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -1523,16 +1521,16 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="A60" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="4" t="s">
+      <c r="D60" t="s">
         <v>13</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -1540,16 +1538,16 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+      <c r="A61" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="4" t="s">
+      <c r="C61" t="s">
         <v>24</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="D61" t="s">
         <v>25</v>
       </c>
       <c r="E61" s="1" t="s">
@@ -1557,16 +1555,16 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+      <c r="A62" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="4" t="s">
+      <c r="D62" t="s">
         <v>11</v>
       </c>
       <c r="E62" s="1" t="s">
@@ -1574,16 +1572,16 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
+      <c r="A63" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C63" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="4" t="s">
+      <c r="D63" t="s">
         <v>11</v>
       </c>
       <c r="E63" s="1" t="s">
@@ -1591,16 +1589,16 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
+      <c r="A64" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" t="s">
         <v>11</v>
       </c>
       <c r="E64" s="1" t="s">
@@ -1608,16 +1606,16 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" t="s">
         <v>10</v>
       </c>
-      <c r="D65" s="4" t="s">
+      <c r="D65" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="1" t="s">
@@ -1625,16 +1623,16 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
+      <c r="A66" t="s">
         <v>5</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" t="s">
         <v>10</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" t="s">
         <v>11</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -1642,16 +1640,16 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
+      <c r="A67" t="s">
         <v>5</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" t="s">
         <v>10</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" t="s">
         <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -1659,16 +1657,16 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="4" t="s">
+      <c r="A68" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" t="s">
         <v>10</v>
       </c>
-      <c r="D68" s="4" t="s">
+      <c r="D68" t="s">
         <v>11</v>
       </c>
       <c r="E68" s="1" t="s">

</xml_diff>

<commit_message>
updated master data with Spanish lang
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/applicant_valid_document.xlsx
+++ b/mosip_master/xlsx/applicant_valid_document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Belize\IJ-CODE\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F907A8E-1C02-46A2-BDC3-ADC0F0F66C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA35E9AB-E37A-4E7C-A5A0-DD1F566EFE8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="23040" windowHeight="12240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -508,13 +508,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="1"/>
-    <col min="5" max="5" width="8.5546875" style="1"/>
+    <col min="2" max="2" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>